<commit_message>
capturing Error messages for unsuccessful login attempts
</commit_message>
<xml_diff>
--- a/src/test/java/com/shopclues/testData/LoginData.xlsx
+++ b/src/test/java/com/shopclues/testData/LoginData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8557D6-303C-4074-81B0-AAD924D0852B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9821435-52EB-46BA-BE83-D87B7D06D0C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8055" yWindow="30" windowWidth="14115" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="30" windowWidth="14115" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -34,16 +34,19 @@
     <t>sasikala.ars@gmail.com</t>
   </si>
   <si>
-    <t>fdsgfh</t>
-  </si>
-  <si>
-    <t>jhjkjhkk</t>
-  </si>
-  <si>
     <t>kgfhjgjhkjk</t>
   </si>
   <si>
     <t>gfhghjgj</t>
+  </si>
+  <si>
+    <t>jhj</t>
+  </si>
+  <si>
+    <t>ewrfethyg</t>
+  </si>
+  <si>
+    <t>tyhjyjthgjnghn</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -461,40 +464,49 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7E862D83-A3A8-4769-A3C9-3B44304F81B6}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{F9C14825-AB9C-40B3-8B0B-E93A512F0559}"/>
+    <hyperlink ref="A4" r:id="rId2" display="sasikala.ars@gmail.com" xr:uid="{F9C14825-AB9C-40B3-8B0B-E93A512F0559}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{2EA10002-7A27-42F2-B515-61993A9C0CDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parallel tests with selenium grid
</commit_message>
<xml_diff>
--- a/src/test/java/com/shopclues/testData/LoginData.xlsx
+++ b/src/test/java/com/shopclues/testData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9821435-52EB-46BA-BE83-D87B7D06D0C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3081E7B7-46CA-4DED-84C2-130FEDCED95F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4785" yWindow="30" windowWidth="14115" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,46 +465,46 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
+      <c r="A3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7E862D83-A3A8-4769-A3C9-3B44304F81B6}"/>
-    <hyperlink ref="A4" r:id="rId2" display="sasikala.ars@gmail.com" xr:uid="{F9C14825-AB9C-40B3-8B0B-E93A512F0559}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{2EA10002-7A27-42F2-B515-61993A9C0CDC}"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{7E862D83-A3A8-4769-A3C9-3B44304F81B6}"/>
+    <hyperlink ref="A3" r:id="rId2" display="sasikala.ars@gmail.com" xr:uid="{F9C14825-AB9C-40B3-8B0B-E93A512F0559}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{2EA10002-7A27-42F2-B515-61993A9C0CDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>